<commit_message>
Listing Reactions for participants
</commit_message>
<xml_diff>
--- a/HackMarathon1/HackMarathon1/Database.xlsx
+++ b/HackMarathon1/HackMarathon1/Database.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\HackMarathon_MechaHU_1\HackMarathon1\HackMarathon1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785C3D60-22BE-4478-8583-98E88617B164}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8F0C8E-9B74-49EE-8682-FADE5CEB033B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="1755" windowWidth="16185" windowHeight="9930" xr2:uid="{A1D49161-1524-4D09-B048-BE6FAC07474B}"/>
+    <workbookView xWindow="32775" yWindow="960" windowWidth="22485" windowHeight="12705" activeTab="1" xr2:uid="{A1D49161-1524-4D09-B048-BE6FAC07474B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>KFC</t>
   </si>
@@ -118,13 +141,37 @@
   </si>
   <si>
     <t>Seafood bistro</t>
+  </si>
+  <si>
+    <t>Cheap</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Reasonable</t>
+  </si>
+  <si>
+    <t>Expensive</t>
+  </si>
+  <si>
+    <t>Misi</t>
+  </si>
+  <si>
+    <t>Gege</t>
+  </si>
+  <si>
+    <t>Bence</t>
+  </si>
+  <si>
+    <t>Heni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,16 +180,36 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -150,12 +217,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -472,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9FCC31-248C-463A-9401-1E81B6AD6D77}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,4 +1100,1426 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFE6330-F91A-4D31-8673-EC53EBBCD833}">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1796875" customWidth="1"/>
+    <col min="15" max="15" width="6.7265625" customWidth="1"/>
+    <col min="16" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>SUM(C2:R2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="0">SUM(C3:R3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <v>1</v>
+      </c>
+      <c r="N13" s="12">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12">
+        <v>0</v>
+      </c>
+      <c r="P13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>0</v>
+      </c>
+      <c r="R13" s="12">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f>SUM(G13:R13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>1</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <v>0</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="12">
+        <v>0</v>
+      </c>
+      <c r="R14" s="12">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ref="S14:S16" si="1">SUM(G14:R14)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12">
+        <v>1</v>
+      </c>
+      <c r="M15" s="12">
+        <v>0</v>
+      </c>
+      <c r="N15" s="12">
+        <v>0</v>
+      </c>
+      <c r="O15" s="12">
+        <v>0</v>
+      </c>
+      <c r="P15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="12">
+        <v>0</v>
+      </c>
+      <c r="R15" s="12">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>1</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <v>1</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="12">
+        <v>0</v>
+      </c>
+      <c r="R16" s="12">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="S17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <f>G13/$S13*$S$17</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" ref="H18:R18" si="2">H13/$S13*$S$17</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" ref="G19:R19" si="3">G14/$S14*$S$17</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" ref="G20:R20" si="4">G15/$S15*$S$17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J20" s="12">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K20" s="12">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L20" s="12">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="12">
+        <f t="shared" ref="G21:R21" si="5">G16/$S16*$S$17</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="12">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1">
+        <v>7</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1">
+        <v>9</v>
+      </c>
+      <c r="L23" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" cm="1">
+        <f t="array" ref="C24:L27">MMULT(C18:R21,TRANSPOSE(C2:R11))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="M24">
+        <f>SUM(C24:L24)</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6">
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="L25" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M27" si="6">SUM(C25:L25)</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1.0033333333333334</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K26" s="6">
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="6"/>
+        <v>6.663333333333334</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G27" s="9">
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="H27" s="9">
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="L27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="6"/>
+        <v>7.4166666666666661</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="C28" s="13">
+        <f>SUM(C24:C27)</f>
+        <v>2.9133333333333331</v>
+      </c>
+      <c r="D28" s="13">
+        <f t="shared" ref="D28:L28" si="7">SUM(D24:D27)</f>
+        <v>2.2466666666666666</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="7"/>
+        <v>2.583333333333333</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="7"/>
+        <v>4.503333333333333</v>
+      </c>
+      <c r="G28" s="13">
+        <f t="shared" si="7"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="H28" s="13">
+        <f t="shared" si="7"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="I28" s="13">
+        <f t="shared" si="7"/>
+        <v>2.17</v>
+      </c>
+      <c r="J28" s="13">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="K28" s="13">
+        <f t="shared" si="7"/>
+        <v>2.9133333333333331</v>
+      </c>
+      <c r="L28" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>